<commit_message>
captcha slover Tesseract & Data Read Write web to excel
</commit_message>
<xml_diff>
--- a/src/test/java/Excel_POI/WriteExcel.xlsx
+++ b/src/test/java/Excel_POI/WriteExcel.xlsx
@@ -63,322 +63,322 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>1.0</v>
+        <v>32.0</v>
       </c>
       <c r="B1" t="n">
-        <v>80.0</v>
+        <v>72.0</v>
       </c>
       <c r="C1" t="n">
-        <v>45.0</v>
+        <v>77.0</v>
       </c>
       <c r="D1" t="n">
-        <v>35.0</v>
+        <v>19.0</v>
       </c>
       <c r="E1" t="n">
-        <v>94.0</v>
+        <v>65.0</v>
       </c>
       <c r="F1" t="n">
-        <v>47.0</v>
+        <v>70.0</v>
       </c>
       <c r="G1" t="n">
-        <v>23.0</v>
+        <v>55.0</v>
       </c>
       <c r="H1" t="n">
-        <v>31.0</v>
+        <v>85.0</v>
       </c>
       <c r="I1" t="n">
-        <v>87.0</v>
+        <v>70.0</v>
       </c>
       <c r="J1" t="n">
-        <v>85.0</v>
+        <v>66.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>58.0</v>
+        <v>16.0</v>
       </c>
       <c r="B2" t="n">
-        <v>94.0</v>
+        <v>81.0</v>
       </c>
       <c r="C2" t="n">
-        <v>11.0</v>
+        <v>63.0</v>
       </c>
       <c r="D2" t="n">
-        <v>81.0</v>
+        <v>75.0</v>
       </c>
       <c r="E2" t="n">
-        <v>80.0</v>
+        <v>17.0</v>
       </c>
       <c r="F2" t="n">
-        <v>96.0</v>
+        <v>57.0</v>
       </c>
       <c r="G2" t="n">
-        <v>21.0</v>
+        <v>26.0</v>
       </c>
       <c r="H2" t="n">
-        <v>4.0</v>
+        <v>71.0</v>
       </c>
       <c r="I2" t="n">
-        <v>50.0</v>
+        <v>10.0</v>
       </c>
       <c r="J2" t="n">
-        <v>56.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>63.0</v>
+        <v>90.0</v>
       </c>
       <c r="B3" t="n">
-        <v>21.0</v>
+        <v>75.0</v>
       </c>
       <c r="C3" t="n">
-        <v>98.0</v>
+        <v>7.0</v>
       </c>
       <c r="D3" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>93.0</v>
+      </c>
+      <c r="H3" t="n">
         <v>51.0</v>
       </c>
-      <c r="E3" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>15.0</v>
-      </c>
       <c r="I3" t="n">
-        <v>62.0</v>
+        <v>89.0</v>
       </c>
       <c r="J3" t="n">
-        <v>28.0</v>
+        <v>89.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>82.0</v>
+        <v>56.0</v>
       </c>
       <c r="B4" t="n">
-        <v>72.0</v>
+        <v>62.0</v>
       </c>
       <c r="C4" t="n">
-        <v>57.0</v>
+        <v>77.0</v>
       </c>
       <c r="D4" t="n">
-        <v>58.0</v>
+        <v>1.0</v>
       </c>
       <c r="E4" t="n">
         <v>59.0</v>
       </c>
       <c r="F4" t="n">
-        <v>73.0</v>
+        <v>40.0</v>
       </c>
       <c r="G4" t="n">
-        <v>57.0</v>
+        <v>19.0</v>
       </c>
       <c r="H4" t="n">
-        <v>28.0</v>
+        <v>76.0</v>
       </c>
       <c r="I4" t="n">
-        <v>33.0</v>
+        <v>89.0</v>
       </c>
       <c r="J4" t="n">
-        <v>57.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>42.0</v>
+        <v>67.0</v>
       </c>
       <c r="B5" t="n">
-        <v>81.0</v>
+        <v>7.0</v>
       </c>
       <c r="C5" t="n">
-        <v>24.0</v>
+        <v>59.0</v>
       </c>
       <c r="D5" t="n">
-        <v>4.0</v>
+        <v>23.0</v>
       </c>
       <c r="E5" t="n">
-        <v>71.0</v>
+        <v>61.0</v>
       </c>
       <c r="F5" t="n">
-        <v>16.0</v>
+        <v>83.0</v>
       </c>
       <c r="G5" t="n">
-        <v>84.0</v>
+        <v>62.0</v>
       </c>
       <c r="H5" t="n">
-        <v>81.0</v>
+        <v>93.0</v>
       </c>
       <c r="I5" t="n">
-        <v>2.0</v>
+        <v>25.0</v>
       </c>
       <c r="J5" t="n">
-        <v>49.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>59.0</v>
+        <v>51.0</v>
       </c>
       <c r="B6" t="n">
-        <v>48.0</v>
+        <v>10.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0</v>
+        <v>73.0</v>
       </c>
       <c r="D6" t="n">
-        <v>53.0</v>
+        <v>73.0</v>
       </c>
       <c r="E6" t="n">
-        <v>23.0</v>
+        <v>45.0</v>
       </c>
       <c r="F6" t="n">
-        <v>45.0</v>
+        <v>43.0</v>
       </c>
       <c r="G6" t="n">
-        <v>96.0</v>
+        <v>93.0</v>
       </c>
       <c r="H6" t="n">
-        <v>47.0</v>
+        <v>36.0</v>
       </c>
       <c r="I6" t="n">
-        <v>1.0</v>
+        <v>28.0</v>
       </c>
       <c r="J6" t="n">
-        <v>19.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>94.0</v>
+        <v>73.0</v>
       </c>
       <c r="B7" t="n">
-        <v>56.0</v>
+        <v>92.0</v>
       </c>
       <c r="C7" t="n">
-        <v>98.0</v>
+        <v>99.0</v>
       </c>
       <c r="D7" t="n">
-        <v>37.0</v>
+        <v>86.0</v>
       </c>
       <c r="E7" t="n">
-        <v>20.0</v>
+        <v>77.0</v>
       </c>
       <c r="F7" t="n">
-        <v>63.0</v>
+        <v>96.0</v>
       </c>
       <c r="G7" t="n">
-        <v>46.0</v>
+        <v>87.0</v>
       </c>
       <c r="H7" t="n">
-        <v>75.0</v>
+        <v>76.0</v>
       </c>
       <c r="I7" t="n">
-        <v>99.0</v>
+        <v>21.0</v>
       </c>
       <c r="J7" t="n">
-        <v>26.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>25.0</v>
+        <v>10.0</v>
       </c>
       <c r="B8" t="n">
-        <v>41.0</v>
+        <v>22.0</v>
       </c>
       <c r="C8" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>92.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="I8" t="n">
         <v>75.0</v>
       </c>
-      <c r="D8" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>82.0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>60.0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>56.0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>50.0</v>
-      </c>
       <c r="J8" t="n">
-        <v>55.0</v>
+        <v>91.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>93.0</v>
+        <v>55.0</v>
       </c>
       <c r="B9" t="n">
-        <v>94.0</v>
+        <v>23.0</v>
       </c>
       <c r="C9" t="n">
-        <v>26.0</v>
+        <v>23.0</v>
       </c>
       <c r="D9" t="n">
-        <v>64.0</v>
+        <v>27.0</v>
       </c>
       <c r="E9" t="n">
-        <v>75.0</v>
+        <v>67.0</v>
       </c>
       <c r="F9" t="n">
-        <v>10.0</v>
+        <v>17.0</v>
       </c>
       <c r="G9" t="n">
-        <v>37.0</v>
+        <v>57.0</v>
       </c>
       <c r="H9" t="n">
-        <v>12.0</v>
+        <v>68.0</v>
       </c>
       <c r="I9" t="n">
-        <v>44.0</v>
+        <v>77.0</v>
       </c>
       <c r="J9" t="n">
-        <v>2.0</v>
+        <v>85.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>49.0</v>
+        <v>28.0</v>
       </c>
       <c r="B10" t="n">
-        <v>17.0</v>
+        <v>43.0</v>
       </c>
       <c r="C10" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="D10" t="n">
         <v>66.0</v>
       </c>
-      <c r="D10" t="n">
-        <v>76.0</v>
-      </c>
       <c r="E10" t="n">
-        <v>71.0</v>
+        <v>56.0</v>
       </c>
       <c r="F10" t="n">
-        <v>9.0</v>
+        <v>72.0</v>
       </c>
       <c r="G10" t="n">
-        <v>82.0</v>
+        <v>55.0</v>
       </c>
       <c r="H10" t="n">
-        <v>9.0</v>
+        <v>86.0</v>
       </c>
       <c r="I10" t="n">
-        <v>19.0</v>
+        <v>78.0</v>
       </c>
       <c r="J10" t="n">
-        <v>38.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>